<commit_message>
update the confiuration files for level2, level3 and level4
</commit_message>
<xml_diff>
--- a/Game/resources/level design.xlsx
+++ b/Game/resources/level design.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yyy\software_engine\2025-group-5\Game\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77803BAB-1A8C-4B35-B477-37874E4243FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12080"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01" sheetId="1" r:id="rId1"/>
@@ -21,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
   <si>
     <t>宝箱</t>
   </si>
@@ -97,18 +101,16 @@
   <si>
     <t>有火附魔，每秒掉血减攻速，持续6s</t>
   </si>
+  <si>
+    <t>玩</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,151 +125,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="9"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,7 +149,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.0999786370433668"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,194 +165,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -567,255 +254,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -891,69 +336,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>43</xdr:col>
@@ -969,13 +373,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1" descr="Dragon_Adventure_01"/>
+        <xdr:cNvPr id="2" name="图片 1" descr="Dragon_Adventure_01">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -996,7 +406,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>41</xdr:col>
@@ -1012,13 +422,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1" descr="Dragon_Adventure_02"/>
+        <xdr:cNvPr id="2" name="图片 1" descr="Dragon_Adventure_02">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1039,7 +455,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>40</xdr:col>
@@ -1055,13 +471,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1092,7 +514,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>40</xdr:col>
@@ -1108,13 +530,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1386,21 +814,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:AN30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.58333333333333" defaultRowHeight="20.15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" customHeight="1" spans="20:40">
+    <row r="4" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -1421,7 +849,7 @@
       <c r="AM4" s="11"/>
       <c r="AN4" s="11"/>
     </row>
-    <row r="5" customHeight="1" spans="14:40">
+    <row r="5" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
@@ -1444,7 +872,7 @@
       <c r="AM5" s="6"/>
       <c r="AN5" s="6"/>
     </row>
-    <row r="6" customHeight="1" spans="14:40">
+    <row r="6" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N6" s="6"/>
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
@@ -1452,7 +880,7 @@
       <c r="AH6" s="6"/>
       <c r="AN6" s="6"/>
     </row>
-    <row r="7" customHeight="1" spans="14:40">
+    <row r="7" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N7" s="11"/>
       <c r="V7" t="s">
         <v>1</v>
@@ -1467,7 +895,7 @@
       <c r="AK7" s="6"/>
       <c r="AN7" s="6"/>
     </row>
-    <row r="8" customHeight="1" spans="14:40">
+    <row r="8" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N8" s="11"/>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
@@ -1480,7 +908,7 @@
       <c r="AL8" s="6"/>
       <c r="AN8" s="6"/>
     </row>
-    <row r="9" customHeight="1" spans="14:40">
+    <row r="9" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N9" s="11"/>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
@@ -1489,7 +917,7 @@
       <c r="Z9" s="6"/>
       <c r="AN9" s="6"/>
     </row>
-    <row r="10" customHeight="1" spans="14:40">
+    <row r="10" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N10" s="11"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
@@ -1503,14 +931,14 @@
       </c>
       <c r="AN10" s="6"/>
     </row>
-    <row r="11" customHeight="1" spans="14:40">
+    <row r="11" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N11" s="11"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="Z11" s="6"/>
       <c r="AN11" s="6"/>
     </row>
-    <row r="12" customHeight="1" spans="3:40">
+    <row r="12" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1525,10 +953,9 @@
       <c r="Q12" s="6"/>
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
-      <c r="AB12"/>
       <c r="AN12" s="6"/>
     </row>
-    <row r="13" customHeight="1" spans="1:40">
+    <row r="13" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1543,7 +970,7 @@
       <c r="AH13" s="6"/>
       <c r="AN13" s="6"/>
     </row>
-    <row r="14" customHeight="1" spans="16:40">
+    <row r="14" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="S14" s="6"/>
@@ -1552,7 +979,7 @@
       <c r="AH14" s="6"/>
       <c r="AN14" s="6"/>
     </row>
-    <row r="15" customHeight="1" spans="16:40">
+    <row r="15" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="S15" s="6"/>
@@ -1561,7 +988,7 @@
       <c r="AH15" s="6"/>
       <c r="AN15" s="6"/>
     </row>
-    <row r="16" customHeight="1" spans="1:40">
+    <row r="16" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="G16" s="6"/>
       <c r="I16" s="6"/>
@@ -1577,7 +1004,7 @@
       <c r="AH16" s="6"/>
       <c r="AN16" s="6"/>
     </row>
-    <row r="17" customHeight="1" spans="1:40">
+    <row r="17" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1590,7 +1017,7 @@
       <c r="AA17" s="6"/>
       <c r="AN17" s="6"/>
     </row>
-    <row r="18" customHeight="1" spans="1:40">
+    <row r="18" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1605,7 +1032,7 @@
       </c>
       <c r="AN18" s="6"/>
     </row>
-    <row r="19" customHeight="1" spans="1:40">
+    <row r="19" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1621,7 +1048,7 @@
       </c>
       <c r="AN19" s="6"/>
     </row>
-    <row r="20" customHeight="1" spans="1:40">
+    <row r="20" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="T20" s="6"/>
@@ -1631,7 +1058,7 @@
       <c r="Z20" s="6"/>
       <c r="AN20" s="6"/>
     </row>
-    <row r="21" customHeight="1" spans="2:40">
+    <row r="21" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="G21" s="6"/>
@@ -1649,7 +1076,7 @@
       <c r="AC21" s="6"/>
       <c r="AN21" s="6"/>
     </row>
-    <row r="22" customHeight="1" spans="3:40">
+    <row r="22" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="6"/>
       <c r="G22" s="6"/>
       <c r="K22" s="6"/>
@@ -1665,7 +1092,7 @@
       <c r="AM22" s="6"/>
       <c r="AN22" s="6"/>
     </row>
-    <row r="23" customHeight="1" spans="3:40">
+    <row r="23" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="G23" s="6"/>
@@ -1682,7 +1109,7 @@
       <c r="AJ23" s="6"/>
       <c r="AN23" s="6"/>
     </row>
-    <row r="24" customHeight="1" spans="4:40">
+    <row r="24" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -1699,7 +1126,7 @@
       <c r="AJ24" s="6"/>
       <c r="AN24" s="6"/>
     </row>
-    <row r="25" customHeight="1" spans="4:40">
+    <row r="25" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="6"/>
       <c r="G25" s="6"/>
       <c r="O25" s="6"/>
@@ -1724,38 +1151,37 @@
       <c r="AM25" s="6"/>
       <c r="AN25" s="6"/>
     </row>
-    <row r="29" customHeight="1" spans="11:11">
+    <row r="29" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" customHeight="1" spans="11:11">
+    <row r="30" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K30" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AN30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y36" sqref="Y36"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="42" width="2.58333333333333" customWidth="1"/>
+    <col min="1" max="42" width="2.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1776,7 +1202,7 @@
       <c r="V1" s="6"/>
       <c r="AN1" s="6"/>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1791,7 +1217,7 @@
       <c r="V2" s="6"/>
       <c r="AN2" s="6"/>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1807,7 +1233,7 @@
       <c r="V3" s="6"/>
       <c r="AN3" s="6"/>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1822,7 +1248,7 @@
       <c r="V4" s="6"/>
       <c r="AN4" s="6"/>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1835,7 +1261,7 @@
       <c r="V5" s="6"/>
       <c r="AN5" s="6"/>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1848,7 +1274,7 @@
       <c r="V6" s="6"/>
       <c r="AN6" s="6"/>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1864,7 +1290,7 @@
       <c r="V7" s="6"/>
       <c r="AN7" s="6"/>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1883,7 +1309,7 @@
       <c r="AG8" s="6"/>
       <c r="AN8" s="6"/>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1903,7 +1329,7 @@
       <c r="AG9" s="6"/>
       <c r="AN9" s="6"/>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1923,7 +1349,7 @@
       <c r="AJ10" s="6"/>
       <c r="AN10" s="6"/>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1952,7 +1378,7 @@
       <c r="AM11" s="6"/>
       <c r="AN11" s="6"/>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1986,7 +1412,7 @@
       <c r="AK12" s="6"/>
       <c r="AN12" s="6"/>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2005,13 +1431,16 @@
       <c r="AH13" s="6"/>
       <c r="AN13" s="6"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:33">
+      <c r="AL14" s="25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -2027,7 +1456,7 @@
       </c>
       <c r="AG15" s="6"/>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2046,7 +1475,7 @@
       <c r="AM16" s="6"/>
       <c r="AN16" s="6"/>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2081,7 +1510,7 @@
       <c r="AM17" s="6"/>
       <c r="AN17" s="6"/>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -2115,7 +1544,7 @@
       <c r="AM18" s="6"/>
       <c r="AN18" s="6"/>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -2143,7 +1572,7 @@
       <c r="AM19" s="6"/>
       <c r="AN19" s="6"/>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -2169,7 +1598,7 @@
       <c r="AM20" s="6"/>
       <c r="AN20" s="6"/>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -2188,7 +1617,7 @@
       <c r="AM21" s="6"/>
       <c r="AN21" s="6"/>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="H22" t="s">
         <v>1</v>
@@ -2215,7 +1644,7 @@
       <c r="AM22" s="6"/>
       <c r="AN22" s="6"/>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="D23" s="6"/>
       <c r="M23" s="6"/>
@@ -2240,7 +1669,7 @@
       <c r="AM23" s="6"/>
       <c r="AN23" s="6"/>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
@@ -2258,7 +1687,7 @@
       <c r="AM24" s="6"/>
       <c r="AN24" s="6"/>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -2286,43 +1715,42 @@
       <c r="AM25" s="6"/>
       <c r="AN25" s="6"/>
     </row>
-    <row r="28" spans="11:11">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="K28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="11:11">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="K29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="11:11">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="K30" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AN39"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="40" width="2.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.75" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2364,7 +1792,7 @@
       <c r="AM1" s="2"/>
       <c r="AN1" s="12"/>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2397,7 +1825,7 @@
       <c r="AM2" s="4"/>
       <c r="AN2" s="13"/>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -2432,7 +1860,7 @@
       <c r="AM3" s="4"/>
       <c r="AN3" s="13"/>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="6"/>
       <c r="E4" s="6"/>
@@ -2465,13 +1893,13 @@
       <c r="AM4" s="11"/>
       <c r="AN4" s="14"/>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="AN5" s="15"/>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2497,7 +1925,7 @@
       <c r="AM6" s="6"/>
       <c r="AN6" s="16"/>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -2525,7 +1953,7 @@
       <c r="AM7" s="4"/>
       <c r="AN7" s="13"/>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2553,7 +1981,7 @@
       <c r="AM8" s="4"/>
       <c r="AN8" s="13"/>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2586,7 +2014,7 @@
       <c r="AM9" s="4"/>
       <c r="AN9" s="13"/>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2616,7 +2044,7 @@
       <c r="AM10" s="4"/>
       <c r="AN10" s="13"/>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="6"/>
       <c r="H11" s="6"/>
@@ -2647,7 +2075,7 @@
       <c r="AM11" s="4"/>
       <c r="AN11" s="13"/>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
       <c r="K12" s="6"/>
@@ -2676,7 +2104,7 @@
       <c r="AM12" s="4"/>
       <c r="AN12" s="13"/>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="6"/>
       <c r="D13" s="6"/>
@@ -2711,7 +2139,7 @@
       <c r="AM13" s="4"/>
       <c r="AN13" s="13"/>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="6"/>
       <c r="D14" s="6"/>
@@ -2748,7 +2176,7 @@
       <c r="AM14" s="4"/>
       <c r="AN14" s="13"/>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="6"/>
       <c r="D15" s="6"/>
@@ -2787,7 +2215,7 @@
       <c r="AM15" s="4"/>
       <c r="AN15" s="16"/>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="6"/>
       <c r="D16" s="6"/>
@@ -2826,7 +2254,7 @@
       <c r="AM16" s="6"/>
       <c r="AN16" s="15"/>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="6"/>
       <c r="D17" s="6"/>
@@ -2866,7 +2294,7 @@
       <c r="AL17" s="6"/>
       <c r="AN17" s="15"/>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="D18" s="6"/>
@@ -2897,7 +2325,7 @@
       <c r="AK18" s="6"/>
       <c r="AN18" s="15"/>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="6"/>
       <c r="D19" s="6"/>
@@ -2923,7 +2351,7 @@
       <c r="AJ19" s="6"/>
       <c r="AN19" s="15"/>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -2949,7 +2377,7 @@
       <c r="AJ20" s="6"/>
       <c r="AN20" s="15"/>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -2977,7 +2405,7 @@
       </c>
       <c r="AN21" s="15"/>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -3004,7 +2432,7 @@
       <c r="AJ22" s="6"/>
       <c r="AN22" s="15"/>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="C23" t="s">
         <v>5</v>
@@ -3017,7 +2445,7 @@
       <c r="W23" s="6"/>
       <c r="AN23" s="15"/>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -3034,7 +2462,7 @@
       <c r="AI24" s="6"/>
       <c r="AN24" s="15"/>
     </row>
-    <row r="25" ht="14.75" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -3076,8 +2504,7 @@
       <c r="AM25" s="21"/>
       <c r="AN25" s="23"/>
     </row>
-    <row r="26" ht="14.75"/>
-    <row r="30" spans="9:14">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="I30" t="s">
         <v>9</v>
       </c>
@@ -3085,7 +2512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="9:14">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
       <c r="I31" t="s">
         <v>10</v>
       </c>
@@ -3093,7 +2520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="9:14">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="I32" t="s">
         <v>11</v>
       </c>
@@ -3104,7 +2531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="9:17">
+    <row r="34" spans="9:17" x14ac:dyDescent="0.2">
       <c r="I34" t="s">
         <v>13</v>
       </c>
@@ -3112,43 +2539,42 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="9:9">
+    <row r="36" spans="9:17" x14ac:dyDescent="0.2">
       <c r="I36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="9:9">
+    <row r="37" spans="9:17" x14ac:dyDescent="0.2">
       <c r="I37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="9:9">
+    <row r="39" spans="9:17" x14ac:dyDescent="0.2">
       <c r="I39" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AN40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="AE41" sqref="AE41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="40" width="2.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.75" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3190,7 +2616,7 @@
       <c r="AM1" s="2"/>
       <c r="AN1" s="12"/>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3232,7 +2658,7 @@
       <c r="AM2" s="4"/>
       <c r="AN2" s="13"/>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3265,7 +2691,7 @@
       <c r="AM3" s="4"/>
       <c r="AN3" s="13"/>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3297,7 +2723,7 @@
       <c r="AM4" s="11"/>
       <c r="AN4" s="14"/>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -3319,7 +2745,7 @@
       <c r="Z5" s="6"/>
       <c r="AN5" s="15"/>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3334,7 +2760,7 @@
       </c>
       <c r="AN6" s="15"/>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3355,7 +2781,7 @@
       <c r="AK7" s="6"/>
       <c r="AN7" s="15"/>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3375,7 +2801,7 @@
       <c r="Z8" s="6"/>
       <c r="AN8" s="15"/>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="J9" s="6"/>
       <c r="N9" s="10"/>
@@ -3399,7 +2825,7 @@
       <c r="AM9" s="6"/>
       <c r="AN9" s="16"/>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="H10" t="s">
         <v>1</v>
@@ -3424,7 +2850,7 @@
       <c r="AM10" s="4"/>
       <c r="AN10" s="13"/>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="N11" s="10"/>
       <c r="X11" s="6"/>
@@ -3440,7 +2866,7 @@
       <c r="AM11" s="4"/>
       <c r="AN11" s="13"/>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -3471,7 +2897,7 @@
       <c r="AM12" s="4"/>
       <c r="AN12" s="13"/>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -3502,7 +2928,7 @@
       <c r="AM13" s="6"/>
       <c r="AN13" s="13"/>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -3526,7 +2952,7 @@
       <c r="AM14" s="6"/>
       <c r="AN14" s="13"/>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -3549,7 +2975,7 @@
       <c r="AM15" s="6"/>
       <c r="AN15" s="13"/>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="4"/>
@@ -3560,7 +2986,7 @@
       <c r="AM16" s="6"/>
       <c r="AN16" s="13"/>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="E17" s="6"/>
       <c r="Q17" s="6"/>
@@ -3573,7 +2999,7 @@
       <c r="AM17" s="6"/>
       <c r="AN17" s="13"/>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="C18" t="s">
         <v>1</v>
@@ -3598,7 +3024,7 @@
       <c r="AM18" s="6"/>
       <c r="AN18" s="13"/>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="4"/>
@@ -3616,7 +3042,7 @@
       <c r="AM19" s="4"/>
       <c r="AN19" s="13"/>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -3646,7 +3072,7 @@
       <c r="AM20" s="4"/>
       <c r="AN20" s="13"/>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -3688,7 +3114,7 @@
       <c r="AM21" s="4"/>
       <c r="AN21" s="13"/>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3730,7 +3156,7 @@
       <c r="AM22" s="4"/>
       <c r="AN22" s="13"/>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3772,7 +3198,7 @@
       <c r="AM23" s="4"/>
       <c r="AN23" s="13"/>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -3814,7 +3240,7 @@
       <c r="AM24" s="4"/>
       <c r="AN24" s="13"/>
     </row>
-    <row r="25" ht="14.75" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -3856,8 +3282,7 @@
       <c r="AM25" s="9"/>
       <c r="AN25" s="17"/>
     </row>
-    <row r="26" ht="14.75"/>
-    <row r="36" spans="15:19">
+    <row r="36" spans="15:19" x14ac:dyDescent="0.2">
       <c r="O36" t="s">
         <v>18</v>
       </c>
@@ -3865,7 +3290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="15:19">
+    <row r="37" spans="15:19" x14ac:dyDescent="0.2">
       <c r="O37" t="s">
         <v>19</v>
       </c>
@@ -3873,7 +3298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="15:19">
+    <row r="38" spans="15:19" x14ac:dyDescent="0.2">
       <c r="O38" t="s">
         <v>20</v>
       </c>
@@ -3881,14 +3306,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="15:15">
+    <row r="40" spans="15:19" x14ac:dyDescent="0.2">
       <c r="O40" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>